<commit_message>
replaced values in excel sheet, commit
</commit_message>
<xml_diff>
--- a/templates/UIfillLead.xlsx
+++ b/templates/UIfillLead.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t xml:space="preserve">Salutation</t>
   </si>
@@ -37,10 +37,10 @@
     <t xml:space="preserve">Ms.</t>
   </si>
   <si>
-    <t xml:space="preserve">Chill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pil</t>
+    <t xml:space="preserve">Pihu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phil</t>
   </si>
   <si>
     <t xml:space="preserve">US</t>
@@ -72,7 +72,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,6 +93,30 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -152,7 +176,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,6 +191,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,18 +212,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="9.91015625" collapsed="true" outlineLevel="0" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="10.23828125" collapsed="true" outlineLevel="0" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="10.12890625" collapsed="true" outlineLevel="0" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="9.57421875" collapsed="true" outlineLevel="0" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" hidden="false" style="1" width="9.91015625" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="1" width="10.23828125" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="1" width="10.12890625" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="1" width="9.57421875" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -231,13 +259,21 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>